<commit_message>
Limmited percentiles to be shown in tab output
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis/output/tables/base_year_benchmark/bench_unbiassdness_e_m.xlsx
+++ b/gdp_revisions_analysis/output/tables/base_year_benchmark/bench_unbiassdness_e_m.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/Research Assistant/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_analysis/output/tables/base_year_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{93F9ABDE-F0F2-437C-8387-4F37526E42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B84553C8-A93F-4ED7-A9DE-87D6053CA958}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{93F9ABDE-F0F2-437C-8387-4F37526E42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9B421B7-179F-4AC4-B2E4-D1757C0F9254}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59A818B8-AC1C-48B4-9EC6-7BF703468C77}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -323,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -348,12 +348,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9546,7 +9540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496513D8-45F4-412F-B325-A911B1FC58A0}">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
@@ -9605,7 +9599,6 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -9635,7 +9628,7 @@
       <c r="I3" s="5">
         <v>3.2</v>
       </c>
-      <c r="J3" s="10"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -9665,7 +9658,7 @@
       <c r="I4" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -9695,7 +9688,7 @@
       <c r="I5" s="2">
         <v>1.8</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -9725,7 +9718,7 @@
       <c r="I6" s="2">
         <v>1.7</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -9755,7 +9748,7 @@
       <c r="I7" s="2">
         <v>1.7</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -9785,7 +9778,7 @@
       <c r="I8" s="2">
         <v>1.6</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -9815,7 +9808,7 @@
       <c r="I9" s="2">
         <v>1.3</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -9845,7 +9838,7 @@
       <c r="I10" s="2">
         <v>1.2</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -9875,7 +9868,7 @@
       <c r="I11" s="2">
         <v>1.2</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -9905,7 +9898,7 @@
       <c r="I12" s="2">
         <v>1.2</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -9935,7 +9928,7 @@
       <c r="I13" s="2">
         <v>0.8</v>
       </c>
-      <c r="J13" s="10"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -9965,7 +9958,7 @@
       <c r="I14" s="2">
         <v>0.6</v>
       </c>
-      <c r="J14" s="10"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -9995,7 +9988,7 @@
       <c r="I15" s="2">
         <v>0.4</v>
       </c>
-      <c r="J15" s="10"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -10025,7 +10018,7 @@
       <c r="I16" s="2">
         <v>0.6</v>
       </c>
-      <c r="J16" s="10"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -10055,7 +10048,7 @@
       <c r="I17" s="2">
         <v>0.6</v>
       </c>
-      <c r="J17" s="10"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -10085,7 +10078,7 @@
       <c r="I18" s="2">
         <v>0.6</v>
       </c>
-      <c r="J18" s="10"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -10115,7 +10108,7 @@
       <c r="I19" s="2">
         <v>0.1</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -10145,7 +10138,7 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="J20" s="10"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -10175,7 +10168,7 @@
       <c r="I21" s="7">
         <v>0</v>
       </c>
-      <c r="J21" s="10"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
@@ -10189,7 +10182,6 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">

</xml_diff>